<commit_message>
Found issue with shared stops
</commit_message>
<xml_diff>
--- a/app/src/test/java/fnsb/macstransit/testfiles/Stops Spreadsheet.xlsx
+++ b/app/src/test/java/fnsb/macstransit/testfiles/Stops Spreadsheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Stephen\Programs\MACSTransitApp\app\src\test\java\fnsb\macstransit\testfiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{079B6458-765C-4B34-8C9D-17E4EFFE8BC5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CD4D3DC-C877-4EF7-A04A-B6C3E5C476C7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-6615" windowWidth="16440" windowHeight="28590" activeTab="2" xr2:uid="{D6478E29-3B83-4DF3-9EB9-29F1C8FC277D}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="3" xr2:uid="{D6478E29-3B83-4DF3-9EB9-29F1C8FC277D}"/>
   </bookViews>
   <sheets>
     <sheet name="Raw stops" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="15">
   <si>
     <t>Blue</t>
   </si>
@@ -80,6 +80,9 @@
   <si>
     <t>Number of stops without duplicates</t>
   </si>
+  <si>
+    <t>Number of shared stops</t>
+  </si>
 </sst>
 </file>
 
@@ -114,8 +117,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -459,38 +465,38 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2" t="s">
+      <c r="B1" s="3"/>
+      <c r="C1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2" t="s">
+      <c r="D1" s="3"/>
+      <c r="E1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2" t="s">
+      <c r="F1" s="3"/>
+      <c r="G1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="H1" s="2"/>
-      <c r="I1" s="2" t="s">
+      <c r="H1" s="3"/>
+      <c r="I1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="2"/>
-      <c r="K1" s="2" t="s">
+      <c r="J1" s="3"/>
+      <c r="K1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="L1" s="2"/>
-      <c r="M1" s="2" t="s">
+      <c r="L1" s="3"/>
+      <c r="M1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="N1" s="2"/>
-      <c r="O1" s="2" t="s">
+      <c r="N1" s="3"/>
+      <c r="O1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="P1" s="2"/>
+      <c r="P1" s="3"/>
     </row>
     <row r="2" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -5827,8 +5833,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3FDFACC0-902C-458B-8401-29B6B3C84D3B}">
   <dimension ref="A1:P106"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="O6" sqref="O6"/>
+    <sheetView topLeftCell="A33" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="M60" sqref="M60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5848,38 +5854,38 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2" t="s">
+      <c r="B1" s="3"/>
+      <c r="C1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2" t="s">
+      <c r="D1" s="3"/>
+      <c r="E1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2" t="s">
+      <c r="F1" s="3"/>
+      <c r="G1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="H1" s="2"/>
-      <c r="I1" s="2" t="s">
+      <c r="H1" s="3"/>
+      <c r="I1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="2"/>
-      <c r="K1" s="2" t="s">
+      <c r="J1" s="3"/>
+      <c r="K1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="L1" s="2"/>
-      <c r="M1" s="2" t="s">
+      <c r="L1" s="3"/>
+      <c r="M1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="N1" s="2"/>
-      <c r="O1" s="2" t="s">
+      <c r="N1" s="3"/>
+      <c r="O1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="P1" s="2"/>
+      <c r="P1" s="3"/>
     </row>
     <row r="2" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -8238,55 +8244,61 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2EB81097-7FEB-436C-8B1E-5D9B58DEE768}">
-  <dimension ref="A1:P6"/>
+  <dimension ref="A1:P18"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G24" sqref="G24"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="M8" sqref="M8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="10" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="10" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11.85546875" customWidth="1"/>
+    <col min="15" max="15" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="11.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2" t="s">
+      <c r="B1" s="3"/>
+      <c r="C1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2" t="s">
+      <c r="D1" s="3"/>
+      <c r="E1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2" t="s">
+      <c r="F1" s="3"/>
+      <c r="G1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="H1" s="2"/>
-      <c r="I1" s="2" t="s">
+      <c r="H1" s="3"/>
+      <c r="I1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="2"/>
-      <c r="K1" s="2" t="s">
+      <c r="J1" s="3"/>
+      <c r="K1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="L1" s="2"/>
-      <c r="M1" s="2" t="s">
+      <c r="L1" s="3"/>
+      <c r="M1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="N1" s="2"/>
-      <c r="O1" s="2" t="s">
+      <c r="N1" s="3"/>
+      <c r="O1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="P1" s="2"/>
+      <c r="P1" s="3"/>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -8345,6 +8357,24 @@
       <c r="B3">
         <v>-147.822067</v>
       </c>
+      <c r="C3">
+        <v>64.840632999999997</v>
+      </c>
+      <c r="D3">
+        <v>-147.72513499999999</v>
+      </c>
+      <c r="G3">
+        <v>64.841434000000007</v>
+      </c>
+      <c r="H3">
+        <v>-147.71964500000001</v>
+      </c>
+      <c r="K3">
+        <v>64.841434000000007</v>
+      </c>
+      <c r="L3">
+        <v>-147.71964500000001</v>
+      </c>
       <c r="M3">
         <v>64.858024</v>
       </c>
@@ -8365,6 +8395,30 @@
       <c r="B4">
         <v>-147.83015599999999</v>
       </c>
+      <c r="C4">
+        <v>64.841434000000007</v>
+      </c>
+      <c r="D4">
+        <v>-147.71964500000001</v>
+      </c>
+      <c r="G4">
+        <v>64.840712999999994</v>
+      </c>
+      <c r="H4">
+        <v>-147.714844</v>
+      </c>
+      <c r="K4">
+        <v>64.840712999999994</v>
+      </c>
+      <c r="L4">
+        <v>-147.714844</v>
+      </c>
+      <c r="M4">
+        <v>64.835809999999995</v>
+      </c>
+      <c r="N4">
+        <v>-147.81517099999999</v>
+      </c>
       <c r="O4">
         <v>64.858011000000005</v>
       </c>
@@ -8379,6 +8433,30 @@
       <c r="B5">
         <v>-147.83503999999999</v>
       </c>
+      <c r="C5">
+        <v>64.857146999999998</v>
+      </c>
+      <c r="D5">
+        <v>-147.69340099999999</v>
+      </c>
+      <c r="G5">
+        <v>64.828755000000001</v>
+      </c>
+      <c r="H5">
+        <v>-147.714787</v>
+      </c>
+      <c r="K5">
+        <v>64.828755000000001</v>
+      </c>
+      <c r="L5">
+        <v>-147.714787</v>
+      </c>
+      <c r="M5">
+        <v>64.841434000000007</v>
+      </c>
+      <c r="N5">
+        <v>-147.71964500000001</v>
+      </c>
       <c r="O5">
         <v>64.858041</v>
       </c>
@@ -8393,11 +8471,305 @@
       <c r="B6">
         <v>-147.84364400000001</v>
       </c>
+      <c r="G6">
+        <v>64.825524999999999</v>
+      </c>
+      <c r="H6">
+        <v>-147.713221</v>
+      </c>
+      <c r="K6">
+        <v>64.825524999999999</v>
+      </c>
+      <c r="L6">
+        <v>-147.713221</v>
+      </c>
+      <c r="M6">
+        <v>64.856099</v>
+      </c>
+      <c r="N6">
+        <v>-147.812825</v>
+      </c>
       <c r="O6">
         <v>64.858110999999994</v>
       </c>
       <c r="P6">
         <v>-147.84364400000001</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>64.858142000000001</v>
+      </c>
+      <c r="B7">
+        <v>-147.850549</v>
+      </c>
+      <c r="G7">
+        <v>64.839010000000002</v>
+      </c>
+      <c r="H7">
+        <v>-147.714099</v>
+      </c>
+      <c r="K7">
+        <v>64.839010000000002</v>
+      </c>
+      <c r="L7">
+        <v>-147.714099</v>
+      </c>
+      <c r="M7">
+        <v>64.863343999999998</v>
+      </c>
+      <c r="N7">
+        <v>-147.81904299999999</v>
+      </c>
+      <c r="O7">
+        <v>64.858142000000001</v>
+      </c>
+      <c r="P7">
+        <v>-147.850549</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>64.847294000000005</v>
+      </c>
+      <c r="B8">
+        <v>-147.81287499999999</v>
+      </c>
+      <c r="G8">
+        <v>64.837226999999999</v>
+      </c>
+      <c r="H8">
+        <v>-147.717251</v>
+      </c>
+      <c r="K8">
+        <v>64.837226999999999</v>
+      </c>
+      <c r="L8">
+        <v>-147.717251</v>
+      </c>
+      <c r="M8">
+        <v>64.860802000000007</v>
+      </c>
+      <c r="N8">
+        <v>-147.822926</v>
+      </c>
+      <c r="O8">
+        <v>64.847294000000005</v>
+      </c>
+      <c r="P8">
+        <v>-147.81287499999999</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>64.843765000000005</v>
+      </c>
+      <c r="B9">
+        <v>-147.81287900000001</v>
+      </c>
+      <c r="G9">
+        <v>64.833945</v>
+      </c>
+      <c r="H9">
+        <v>-147.71713</v>
+      </c>
+      <c r="K9">
+        <v>64.833945</v>
+      </c>
+      <c r="L9">
+        <v>-147.71713</v>
+      </c>
+      <c r="M9">
+        <v>64.857146999999998</v>
+      </c>
+      <c r="N9">
+        <v>-147.69340099999999</v>
+      </c>
+      <c r="O9">
+        <v>64.843765000000005</v>
+      </c>
+      <c r="P9">
+        <v>-147.81287900000001</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>64.837947999999997</v>
+      </c>
+      <c r="B10">
+        <v>-147.812816</v>
+      </c>
+      <c r="G10">
+        <v>64.831175999999999</v>
+      </c>
+      <c r="H10">
+        <v>-147.715881</v>
+      </c>
+      <c r="K10">
+        <v>64.831175999999999</v>
+      </c>
+      <c r="L10">
+        <v>-147.715881</v>
+      </c>
+      <c r="M10">
+        <v>64.838026999999997</v>
+      </c>
+      <c r="N10">
+        <v>-147.812386</v>
+      </c>
+      <c r="O10">
+        <v>64.837947999999997</v>
+      </c>
+      <c r="P10">
+        <v>-147.812816</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>64.835809999999995</v>
+      </c>
+      <c r="B11">
+        <v>-147.81517099999999</v>
+      </c>
+      <c r="G11">
+        <v>64.822730000000007</v>
+      </c>
+      <c r="H11">
+        <v>-147.71213499999999</v>
+      </c>
+      <c r="K11">
+        <v>64.822730000000007</v>
+      </c>
+      <c r="L11">
+        <v>-147.71213499999999</v>
+      </c>
+      <c r="M11">
+        <v>64.844121999999999</v>
+      </c>
+      <c r="N11">
+        <v>-147.81242700000001</v>
+      </c>
+      <c r="O11">
+        <v>64.835809999999995</v>
+      </c>
+      <c r="P11">
+        <v>-147.81517099999999</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>64.840632999999997</v>
+      </c>
+      <c r="B12">
+        <v>-147.72513499999999</v>
+      </c>
+      <c r="G12">
+        <v>64.838575000000006</v>
+      </c>
+      <c r="H12">
+        <v>-147.71881500000001</v>
+      </c>
+      <c r="K12">
+        <v>64.838575000000006</v>
+      </c>
+      <c r="L12">
+        <v>-147.71881500000001</v>
+      </c>
+      <c r="M12">
+        <v>64.847216000000003</v>
+      </c>
+      <c r="N12">
+        <v>-147.812431</v>
+      </c>
+      <c r="O12">
+        <v>64.856099</v>
+      </c>
+      <c r="P12">
+        <v>-147.812825</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>64.841434000000007</v>
+      </c>
+      <c r="B13">
+        <v>-147.71964500000001</v>
+      </c>
+      <c r="M13">
+        <v>64.849359000000007</v>
+      </c>
+      <c r="N13">
+        <v>-147.812431</v>
+      </c>
+      <c r="O13">
+        <v>64.863343999999998</v>
+      </c>
+      <c r="P13">
+        <v>-147.81904299999999</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>64.856099</v>
+      </c>
+      <c r="B14">
+        <v>-147.812825</v>
+      </c>
+      <c r="M14">
+        <v>64.851911999999999</v>
+      </c>
+      <c r="N14">
+        <v>-147.81247400000001</v>
+      </c>
+      <c r="O14">
+        <v>64.860802000000007</v>
+      </c>
+      <c r="P14">
+        <v>-147.822926</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>64.863343999999998</v>
+      </c>
+      <c r="B15">
+        <v>-147.81904299999999</v>
+      </c>
+      <c r="O15">
+        <v>64.838026999999997</v>
+      </c>
+      <c r="P15">
+        <v>-147.812386</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>64.860802000000007</v>
+      </c>
+      <c r="B16">
+        <v>-147.822926</v>
+      </c>
+      <c r="O16">
+        <v>64.844121999999999</v>
+      </c>
+      <c r="P16">
+        <v>-147.81242700000001</v>
+      </c>
+    </row>
+    <row r="17" spans="15:16" x14ac:dyDescent="0.25">
+      <c r="O17">
+        <v>64.847216000000003</v>
+      </c>
+      <c r="P17">
+        <v>-147.812431</v>
+      </c>
+    </row>
+    <row r="18" spans="15:16" x14ac:dyDescent="0.25">
+      <c r="O18">
+        <v>64.849359000000007</v>
+      </c>
+      <c r="P18">
+        <v>-147.812431</v>
       </c>
     </row>
   </sheetData>
@@ -8417,10 +8789,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5BCD8F6B-1C7A-45E3-9213-D5AF40D2D617}">
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8428,9 +8800,10 @@
     <col min="1" max="1" width="10.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="30.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="33.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>11</v>
       </c>
@@ -8440,22 +8813,29 @@
       <c r="C1" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="str">
         <f>'Raw stops'!A1</f>
         <v>Blue</v>
       </c>
       <c r="B2" s="1">
-        <f>COUNT('Raw stops'!A3:A235)</f>
+        <f>COUNT('Raw stops'!$A3:$A235)</f>
         <v>233</v>
       </c>
       <c r="C2" s="1">
         <f>COUNT('All Stops'!A3:A235)</f>
         <v>66</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D2" s="2">
+        <f>COUNT('Shared Stops'!A$3:A$235)</f>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="str">
         <f>'Raw stops'!C1</f>
         <v>Brown</v>
@@ -8468,8 +8848,12 @@
         <f>COUNT('All Stops'!D3:D26)</f>
         <v>24</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D3" s="2">
+        <f>COUNT('Shared Stops'!C$3:C$235)</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="str">
         <f>'Raw stops'!E1</f>
         <v>Gray</v>
@@ -8482,8 +8866,12 @@
         <f>COUNT('All Stops'!F3:F235)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D4" s="2">
+        <f>COUNT('Shared Stops'!E$3:E$235)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="str">
         <f>'Raw stops'!G1</f>
         <v>Green</v>
@@ -8496,8 +8884,12 @@
         <f>COUNT('All Stops'!H3:H146)</f>
         <v>104</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D5" s="2">
+        <f>COUNT('Shared Stops'!G$3:G$235)</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="str">
         <f>'Raw stops'!I1</f>
         <v>Orange</v>
@@ -8510,8 +8902,12 @@
         <f>COUNT('All Stops'!J3:J235)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D6" s="2">
+        <f>COUNT('Shared Stops'!I$3:I$235)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="str">
         <f>'Raw stops'!K1</f>
         <v>Purple</v>
@@ -8524,8 +8920,12 @@
         <f>COUNT('All Stops'!L3:L80)</f>
         <v>39</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D7" s="2">
+        <f>COUNT('Shared Stops'!K$3:K$235)</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="str">
         <f>'Raw stops'!M1</f>
         <v>Red</v>
@@ -8538,8 +8938,12 @@
         <f>COUNT('All Stops'!N3:N178)</f>
         <v>58</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D8" s="2">
+        <f>COUNT('Shared Stops'!M$3:M$235)</f>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="str">
         <f>'Raw stops'!O1</f>
         <v>Yellow</v>
@@ -8552,8 +8956,15 @@
         <f>COUNT('All Stops'!P3:P147)</f>
         <v>56</v>
       </c>
+      <c r="D9" s="2">
+        <f>COUNT('Shared Stops'!O$3:O$235)</f>
+        <v>16</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <ignoredErrors>
+    <ignoredError sqref="D3" formula="1"/>
+  </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Validated shared stop removal
</commit_message>
<xml_diff>
--- a/app/src/test/java/fnsb/macstransit/testfiles/Stops Spreadsheet.xlsx
+++ b/app/src/test/java/fnsb/macstransit/testfiles/Stops Spreadsheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Stephen\Programs\MACSTransitApp\app\src\test\java\fnsb\macstransit\testfiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CD4D3DC-C877-4EF7-A04A-B6C3E5C476C7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B055DD5-99D0-43D2-9EF1-9EE23310AA93}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="3" xr2:uid="{D6478E29-3B83-4DF3-9EB9-29F1C8FC277D}"/>
+    <workbookView xWindow="28680" yWindow="-6615" windowWidth="16440" windowHeight="28590" activeTab="3" xr2:uid="{D6478E29-3B83-4DF3-9EB9-29F1C8FC277D}"/>
   </bookViews>
   <sheets>
     <sheet name="Raw stops" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="16">
   <si>
     <t>Blue</t>
   </si>
@@ -83,6 +83,9 @@
   <si>
     <t>Number of shared stops</t>
   </si>
+  <si>
+    <t>Final stop count</t>
+  </si>
 </sst>
 </file>
 
@@ -117,8 +120,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -465,38 +471,38 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3" t="s">
+      <c r="B1" s="4"/>
+      <c r="C1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3" t="s">
+      <c r="D1" s="4"/>
+      <c r="E1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="F1" s="3"/>
-      <c r="G1" s="3" t="s">
+      <c r="F1" s="4"/>
+      <c r="G1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="H1" s="3"/>
-      <c r="I1" s="3" t="s">
+      <c r="H1" s="4"/>
+      <c r="I1" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="3"/>
-      <c r="K1" s="3" t="s">
+      <c r="J1" s="4"/>
+      <c r="K1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="L1" s="3"/>
-      <c r="M1" s="3" t="s">
+      <c r="L1" s="4"/>
+      <c r="M1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="N1" s="3"/>
-      <c r="O1" s="3" t="s">
+      <c r="N1" s="4"/>
+      <c r="O1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="P1" s="3"/>
+      <c r="P1" s="4"/>
     </row>
     <row r="2" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -5833,8 +5839,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3FDFACC0-902C-458B-8401-29B6B3C84D3B}">
   <dimension ref="A1:P106"/>
   <sheetViews>
-    <sheetView topLeftCell="A33" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M60" sqref="M60"/>
+    <sheetView topLeftCell="A2" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="M66" sqref="M66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5854,38 +5860,38 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3" t="s">
+      <c r="B1" s="4"/>
+      <c r="C1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3" t="s">
+      <c r="D1" s="4"/>
+      <c r="E1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="F1" s="3"/>
-      <c r="G1" s="3" t="s">
+      <c r="F1" s="4"/>
+      <c r="G1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="H1" s="3"/>
-      <c r="I1" s="3" t="s">
+      <c r="H1" s="4"/>
+      <c r="I1" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="3"/>
-      <c r="K1" s="3" t="s">
+      <c r="J1" s="4"/>
+      <c r="K1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="L1" s="3"/>
-      <c r="M1" s="3" t="s">
+      <c r="L1" s="4"/>
+      <c r="M1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="N1" s="3"/>
-      <c r="O1" s="3" t="s">
+      <c r="N1" s="4"/>
+      <c r="O1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="P1" s="3"/>
+      <c r="P1" s="4"/>
     </row>
     <row r="2" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -8244,10 +8250,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2EB81097-7FEB-436C-8B1E-5D9B58DEE768}">
-  <dimension ref="A1:P18"/>
+  <dimension ref="A1:P19"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M8" sqref="M8"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8267,38 +8273,38 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3" t="s">
+      <c r="B1" s="4"/>
+      <c r="C1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3" t="s">
+      <c r="D1" s="4"/>
+      <c r="E1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="F1" s="3"/>
-      <c r="G1" s="3" t="s">
+      <c r="F1" s="4"/>
+      <c r="G1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="H1" s="3"/>
-      <c r="I1" s="3" t="s">
+      <c r="H1" s="4"/>
+      <c r="I1" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="3"/>
-      <c r="K1" s="3" t="s">
+      <c r="J1" s="4"/>
+      <c r="K1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="L1" s="3"/>
-      <c r="M1" s="3" t="s">
+      <c r="L1" s="4"/>
+      <c r="M1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="N1" s="3"/>
-      <c r="O1" s="3" t="s">
+      <c r="N1" s="4"/>
+      <c r="O1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="P1" s="3"/>
+      <c r="P1" s="4"/>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -8770,6 +8776,14 @@
       </c>
       <c r="P18">
         <v>-147.812431</v>
+      </c>
+    </row>
+    <row r="19" spans="15:16" x14ac:dyDescent="0.25">
+      <c r="O19">
+        <v>64.851911999999999</v>
+      </c>
+      <c r="P19">
+        <v>-147.81247400000001</v>
       </c>
     </row>
   </sheetData>
@@ -8789,10 +8803,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5BCD8F6B-1C7A-45E3-9213-D5AF40D2D617}">
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8801,9 +8815,10 @@
     <col min="2" max="2" width="30.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="33.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="22.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>11</v>
       </c>
@@ -8816,8 +8831,11 @@
       <c r="D1" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="str">
         <f>'Raw stops'!A1</f>
         <v>Blue</v>
@@ -8834,8 +8852,12 @@
         <f>COUNT('Shared Stops'!A$3:A$235)</f>
         <v>14</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E2" s="3">
+        <f>C2-D2</f>
+        <v>52</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="str">
         <f>'Raw stops'!C1</f>
         <v>Brown</v>
@@ -8852,8 +8874,12 @@
         <f>COUNT('Shared Stops'!C$3:C$235)</f>
         <v>3</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E3" s="3">
+        <f t="shared" ref="E3:E9" si="0">C3-D3</f>
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="str">
         <f>'Raw stops'!E1</f>
         <v>Gray</v>
@@ -8870,8 +8896,12 @@
         <f>COUNT('Shared Stops'!E$3:E$235)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E4" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="str">
         <f>'Raw stops'!G1</f>
         <v>Green</v>
@@ -8888,8 +8918,12 @@
         <f>COUNT('Shared Stops'!G$3:G$235)</f>
         <v>10</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E5" s="3">
+        <f t="shared" si="0"/>
+        <v>94</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="str">
         <f>'Raw stops'!I1</f>
         <v>Orange</v>
@@ -8906,8 +8940,12 @@
         <f>COUNT('Shared Stops'!I$3:I$235)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E6" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="str">
         <f>'Raw stops'!K1</f>
         <v>Purple</v>
@@ -8924,8 +8962,12 @@
         <f>COUNT('Shared Stops'!K$3:K$235)</f>
         <v>10</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E7" s="3">
+        <f t="shared" si="0"/>
+        <v>29</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="str">
         <f>'Raw stops'!M1</f>
         <v>Red</v>
@@ -8942,8 +8984,12 @@
         <f>COUNT('Shared Stops'!M$3:M$235)</f>
         <v>12</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E8" s="3">
+        <f t="shared" si="0"/>
+        <v>46</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="str">
         <f>'Raw stops'!O1</f>
         <v>Yellow</v>
@@ -8958,7 +9004,11 @@
       </c>
       <c r="D9" s="2">
         <f>COUNT('Shared Stops'!O$3:O$235)</f>
-        <v>16</v>
+        <v>17</v>
+      </c>
+      <c r="E9" s="3">
+        <f t="shared" si="0"/>
+        <v>39</v>
       </c>
     </row>
   </sheetData>

</xml_diff>